<commit_message>
Headless mode test commit
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/LoginTestData.xlsx
+++ b/src/test/resources/testData/LoginTestData.xlsx
@@ -2,16 +2,36 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
-  <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{451697CB-59A4-4A1E-9D11-005A92DAF65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5ed14a977c71b691/Desktop/TekArch/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{A8384708-A205-4D05-9226-285DEBEC5AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC68BB5B-BB8C-47EA-9BD0-83E0C0B22EB9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9C3CA171-213A-41B0-83FF-F1BFEF12DEDE}"/>
   </bookViews>
   <sheets>
     <sheet name="UserCreds" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -33,13 +53,13 @@
     <t>Sumedh@03</t>
   </si>
   <si>
+    <t>Sumedh</t>
+  </si>
+  <si>
     <t>anusha@tek</t>
   </si>
   <si>
     <t>anusha@t.com</t>
-  </si>
-  <si>
-    <t>Sumedh</t>
   </si>
   <si>
     <t>Anusha</t>
@@ -49,24 +69,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -87,18 +95,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -115,56 +118,150 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -307,89 +404,85 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F8DFD7C-DEE8-49E9-924F-5DB820517369}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{0F1F8774-94B7-4A93-8D7D-0894425986A5}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{243D30A1-D44E-4E4C-9CED-6F986B015362}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{20767A19-8E96-4891-8F93-F0E1E36CBD03}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{AD16C0D9-BBB3-46EB-A0B6-A48E8B509984}"/>
-    <hyperlink ref="C3" r:id="rId5" display="Sumedh@03" xr:uid="{0490204A-6D80-4585-A921-A19A67FC51D7}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{21EFB6F0-602B-4569-AE30-7392A6E6D08E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes made while reading excel file. commented wb.close file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/LoginTestData.xlsx
+++ b/src/test/resources/testData/LoginTestData.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5ed14a977c71b691/Desktop/TekArch/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A8384708-A205-4D05-9226-285DEBEC5AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC68BB5B-BB8C-47EA-9BD0-83E0C0B22EB9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FAAEFAA9-433C-4CEA-8D50-7A59A7CFC822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9C3CA171-213A-41B0-83FF-F1BFEF12DEDE}"/>
   </bookViews>
   <sheets>
     <sheet name="UserCreds" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>